<commit_message>
Fix typo in Master.xlsx
</commit_message>
<xml_diff>
--- a/Master.xlsx
+++ b/Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\Project\Golang\JadwalPetugas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960E4941-AB9E-4F5E-9578-C97C8E2B527A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40B6D94-4F13-4A44-BF4D-7EAE272EFCE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Petugas" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>Pnt. Anita Sarl</t>
-  </si>
-  <si>
     <t>Pnt. Chrismas Dikywidhiyana</t>
   </si>
   <si>
@@ -299,6 +296,9 @@
   </si>
   <si>
     <t>Kolektan 4</t>
+  </si>
+  <si>
+    <t>Pnt. Anita Sari</t>
   </si>
 </sst>
 </file>
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -668,7 +668,7 @@
         <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>2</v>
@@ -703,7 +703,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
@@ -727,7 +727,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -751,7 +751,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -775,7 +775,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -797,7 +797,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -819,7 +819,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -841,7 +841,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -865,7 +865,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
@@ -885,7 +885,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
@@ -905,7 +905,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
@@ -929,7 +929,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
@@ -949,7 +949,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
@@ -969,7 +969,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
@@ -989,7 +989,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
@@ -1011,7 +1011,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
@@ -1031,7 +1031,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
@@ -1051,7 +1051,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
@@ -1071,7 +1071,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
@@ -1093,7 +1093,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
@@ -1115,7 +1115,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
@@ -1137,7 +1137,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
@@ -1159,7 +1159,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
@@ -1181,7 +1181,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
@@ -1203,7 +1203,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
@@ -1225,7 +1225,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
@@ -1247,7 +1247,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1267,7 +1267,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1287,7 +1287,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
@@ -1307,7 +1307,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1325,7 +1325,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
@@ -1345,7 +1345,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
@@ -1365,7 +1365,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1383,7 +1383,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1401,7 +1401,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1419,7 +1419,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1437,7 +1437,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
@@ -1457,7 +1457,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
@@ -1477,7 +1477,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
@@ -2249,7 +2249,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -2284,7 +2284,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -2304,7 +2304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC7D8F8-943A-4461-BBC0-7DFF79EB9EEA}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -2318,13 +2318,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="C1" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
@@ -2335,7 +2335,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
@@ -2346,7 +2346,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
@@ -2357,205 +2357,205 @@
         <v>2</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
@@ -2566,29 +2566,29 @@
         <v>11</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2632,17 +2632,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>